<commit_message>
Complete 2018-2018 tables for submission.
</commit_message>
<xml_diff>
--- a/parameters/pcode_table_FINAL_CODES_2020-08-28.xlsx
+++ b/parameters/pcode_table_FINAL_CODES_2020-08-28.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\its_data_modernization_local\chem_hist_cleaning\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE60ABCA-98CB-4F7D-AF6C-223DB5183504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C44BB2E-5A77-4F88-B2AF-053CBF694D97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ED1AB139-CA79-4663-894E-917D94973C31}"/>
   </bookViews>
@@ -2297,8 +2297,8 @@
   <dimension ref="A1:S167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>